<commit_message>
Update demo project with enhanced waiting times, filter and improvements
</commit_message>
<xml_diff>
--- a/assets/export.template.xlsx
+++ b/assets/export.template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\trip.tracker\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A6A77-F331-42B5-A7C3-841378D3F47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED22C36-8E33-4B8E-8A2F-4BDC04B1DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>%date%</t>
   </si>
@@ -48,31 +48,46 @@
     <t>%start%</t>
   </si>
   <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>Dienstbeginn</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Dienstende</t>
+  </si>
+  <si>
+    <t>Abfahrt / Ankunft</t>
+  </si>
+  <si>
+    <t>Gastfahrt nach Dienstende</t>
+  </si>
+  <si>
+    <t>Bemerkungen</t>
+  </si>
+  <si>
+    <t>Wartezeit 1</t>
+  </si>
+  <si>
+    <t>Wartezeit 2</t>
+  </si>
+  <si>
+    <t>Pause Gesamt</t>
+  </si>
+  <si>
+    <t>Gesamt Dienststunden</t>
+  </si>
+  <si>
+    <t>Dienstbeginn Ort</t>
+  </si>
+  <si>
+    <t>Dienstende Ort</t>
+  </si>
+  <si>
     <t>Gastfahrt vor Dienstbeginn</t>
-  </si>
-  <si>
-    <t>Gesamt</t>
-  </si>
-  <si>
-    <t>Dienstbeginn</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>Dienstende</t>
-  </si>
-  <si>
-    <t>Abfahrt / Ankunft</t>
-  </si>
-  <si>
-    <t>Gesamt Dienststd.</t>
-  </si>
-  <si>
-    <t>Gastfahrt nach Dienstende</t>
-  </si>
-  <si>
-    <t>Bemerkungen</t>
   </si>
 </sst>
 </file>
@@ -390,43 +405,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.7265625" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.7265625" customWidth="1"/>
+    <col min="6" max="9" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -437,37 +454,55 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="Q5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
         <v>13</v>
       </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Upload new version 1.0.0
</commit_message>
<xml_diff>
--- a/assets/export.template.xlsx
+++ b/assets/export.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\trip.tracker\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED22C36-8E33-4B8E-8A2F-4BDC04B1DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58FBBF4-B54F-4FC1-B5E9-3B7E647C9602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>%date%</t>
   </si>
@@ -54,27 +54,12 @@
     <t>Dienstbeginn</t>
   </si>
   <si>
-    <t>Pause</t>
-  </si>
-  <si>
     <t>Dienstende</t>
   </si>
   <si>
-    <t>Abfahrt / Ankunft</t>
-  </si>
-  <si>
-    <t>Gastfahrt nach Dienstende</t>
-  </si>
-  <si>
     <t>Bemerkungen</t>
   </si>
   <si>
-    <t>Wartezeit 1</t>
-  </si>
-  <si>
-    <t>Wartezeit 2</t>
-  </si>
-  <si>
     <t>Pause Gesamt</t>
   </si>
   <si>
@@ -87,7 +72,43 @@
     <t>Dienstende Ort</t>
   </si>
   <si>
-    <t>Gastfahrt vor Dienstbeginn</t>
+    <t>Pause von</t>
+  </si>
+  <si>
+    <t>Pause bis</t>
+  </si>
+  <si>
+    <t>Wartezeit 1 von</t>
+  </si>
+  <si>
+    <t>Wartezeit 1 bis</t>
+  </si>
+  <si>
+    <t>Wartezeit 2 von</t>
+  </si>
+  <si>
+    <t>Wartezeit 2 bis</t>
+  </si>
+  <si>
+    <t>Abfahrt</t>
+  </si>
+  <si>
+    <t>Ankunft</t>
+  </si>
+  <si>
+    <t>Gastfahrt vor Dienstbeginn von</t>
+  </si>
+  <si>
+    <t>Gastfahrt vor Dienstbeginn bis</t>
+  </si>
+  <si>
+    <t>Gastfahrt nach Dienstende von</t>
+  </si>
+  <si>
+    <t>Gastfahrt nach Dienstende bis</t>
+  </si>
+  <si>
+    <t>Zugnummer</t>
   </si>
 </sst>
 </file>
@@ -405,45 +426,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="9" width="15.1796875" customWidth="1"/>
-    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" customWidth="1"/>
+    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -451,25 +473,25 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
@@ -478,31 +500,52 @@
         <v>16</v>
       </c>
       <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" t="s">
+        <v>7</v>
+      </c>
+      <c r="V5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W5" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z5" t="s">
         <v>10</v>
       </c>
-      <c r="M5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>7</v>
-      </c>
-      <c r="R5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>